<commit_message>
[lab5] remove extra rows
</commit_message>
<xml_diff>
--- a/lab5/task3/SolutionsTable.xlsx
+++ b/lab5/task3/SolutionsTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pk_er\Projects\Projects_C#\TiOPO-labs\lab5\task3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB53872E-AC10-431A-95BC-9C36D7EAF7B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80614419-985D-48E1-A2EC-06B15175DF4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{355B0D5D-F77B-43F9-8C0A-DDB77AC0C27B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{355B0D5D-F77B-43F9-8C0A-DDB77AC0C27B}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="20">
   <si>
     <t>Условие</t>
   </si>
@@ -118,7 +118,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,12 +139,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -152,6 +146,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF66CC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,22 +174,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF66CC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -492,20 +504,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A3B8D3E-83F9-4130-A151-C249913B47DF}">
-  <dimension ref="A1:AI44"/>
+  <dimension ref="A1:AI36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="N42" sqref="N42"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.6640625" customWidth="1"/>
-    <col min="35" max="35" width="29.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="35" max="35" width="29.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -548,7 +560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -655,7 +667,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -762,7 +774,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -869,7 +881,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -976,7 +988,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1083,7 +1095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1190,7 +1202,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1297,7 +1309,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1511,12 +1523,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>17</v>
       </c>
@@ -1617,7 +1629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>3</v>
       </c>
@@ -1708,7 +1720,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -1788,7 +1800,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>5</v>
       </c>
@@ -1868,7 +1880,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -1948,7 +1960,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -2108,7 +2120,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="21" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -2188,7 +2200,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -2268,7 +2280,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -2348,1111 +2360,419 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C26" s="9">
+        <v>0</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I26" s="6">
+        <v>1</v>
+      </c>
+      <c r="J26" s="6">
+        <v>1</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L26" s="4"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="4"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="4"/>
+      <c r="R26" s="4"/>
+      <c r="S26" s="4"/>
+    </row>
+    <row r="27" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" s="9">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="5">
+        <v>1</v>
+      </c>
+      <c r="H27" s="5">
+        <v>1</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0</v>
+      </c>
+      <c r="J27" s="6">
+        <v>0</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+    </row>
+    <row r="28" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>5</v>
+      </c>
+      <c r="C28" s="9">
+        <v>0</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0</v>
+      </c>
+      <c r="E28" s="3">
+        <v>1</v>
+      </c>
+      <c r="F28" s="3">
+        <v>1</v>
+      </c>
+      <c r="G28" s="5">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5">
+        <v>0</v>
+      </c>
+      <c r="I28" s="6">
+        <v>0</v>
+      </c>
+      <c r="J28" s="6">
+        <v>0</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L28" s="4"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+    </row>
+    <row r="29" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C29" s="9">
+        <v>1</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0</v>
+      </c>
+      <c r="E29" s="3">
+        <v>1</v>
+      </c>
+      <c r="F29" s="3">
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <v>1</v>
+      </c>
+      <c r="H29" s="5">
+        <v>0</v>
+      </c>
+      <c r="I29" s="6">
+        <v>1</v>
+      </c>
+      <c r="J29" s="6">
+        <v>0</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+    </row>
+    <row r="30" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>0</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0</v>
+      </c>
+      <c r="F30" s="3">
+        <v>0</v>
+      </c>
+      <c r="G30" s="5">
+        <v>0</v>
+      </c>
+      <c r="H30" s="5">
+        <v>0</v>
+      </c>
+      <c r="I30" s="6">
+        <v>0</v>
+      </c>
+      <c r="J30" s="6">
+        <v>0</v>
+      </c>
+      <c r="K30" s="8">
+        <v>1</v>
+      </c>
+      <c r="L30" s="4"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="4"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="4"/>
+      <c r="Q30" s="4"/>
+      <c r="R30" s="4"/>
+      <c r="S30" s="4"/>
+    </row>
+    <row r="31" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="C31" s="9">
+        <v>0</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0</v>
+      </c>
+      <c r="F31" s="3">
+        <v>0</v>
+      </c>
+      <c r="G31" s="5">
+        <v>0</v>
+      </c>
+      <c r="H31" s="5">
+        <v>0</v>
+      </c>
+      <c r="I31" s="6">
+        <v>3</v>
+      </c>
+      <c r="J31" s="6">
+        <v>3</v>
+      </c>
+      <c r="K31" s="8">
+        <v>0</v>
+      </c>
+      <c r="L31" s="4"/>
+      <c r="M31" s="4"/>
+      <c r="N31" s="4"/>
+      <c r="O31" s="4"/>
+      <c r="P31" s="4"/>
+      <c r="Q31" s="4"/>
+      <c r="R31" s="4"/>
+      <c r="S31" s="4"/>
+    </row>
+    <row r="32" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="C32" s="9">
+        <v>0</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0</v>
+      </c>
+      <c r="F32" s="3">
+        <v>0</v>
+      </c>
+      <c r="G32" s="5">
+        <v>10</v>
+      </c>
+      <c r="H32" s="5">
+        <v>10</v>
+      </c>
+      <c r="I32" s="6">
+        <v>0</v>
+      </c>
+      <c r="J32" s="6">
+        <v>0</v>
+      </c>
+      <c r="K32" s="8">
+        <v>0</v>
+      </c>
+      <c r="L32" s="4"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="4"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="4"/>
+      <c r="Q32" s="4"/>
+      <c r="R32" s="4"/>
+      <c r="S32" s="4"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" s="9">
+        <v>0</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0</v>
+      </c>
+      <c r="E33" s="3">
+        <v>12</v>
+      </c>
+      <c r="F33" s="3">
+        <v>12</v>
+      </c>
+      <c r="G33" s="5">
+        <v>0</v>
+      </c>
+      <c r="H33" s="5">
+        <v>0</v>
+      </c>
+      <c r="I33" s="6">
+        <v>0</v>
+      </c>
+      <c r="J33" s="6">
+        <v>0</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0</v>
+      </c>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" s="9">
+        <v>5</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0</v>
+      </c>
+      <c r="E34" s="3">
+        <v>5</v>
+      </c>
+      <c r="F34" s="3">
+        <v>0</v>
+      </c>
+      <c r="G34" s="5">
+        <v>5</v>
+      </c>
+      <c r="H34" s="5">
+        <v>0</v>
+      </c>
+      <c r="I34" s="6">
+        <v>5</v>
+      </c>
+      <c r="J34" s="6">
+        <v>0</v>
+      </c>
+      <c r="K34" s="8">
+        <v>0</v>
+      </c>
+      <c r="L34" s="4"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="4"/>
+      <c r="R34" s="4"/>
+      <c r="S34" s="4"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>17</v>
+      </c>
+      <c r="C36">
+        <f t="shared" ref="C36:D36" si="0">SUM(C31:C34)</f>
+        <v>5</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <f>SUM(E31:E34)</f>
+        <v>17</v>
+      </c>
+      <c r="F36">
+        <f t="shared" ref="F36:K36" si="1">SUM(F31:F34)</f>
+        <v>12</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C24" s="4">
-        <v>0</v>
-      </c>
-      <c r="D24" s="4">
-        <v>0</v>
-      </c>
-      <c r="E24" s="4">
-        <v>0</v>
-      </c>
-      <c r="F24" s="3">
-        <v>0</v>
-      </c>
-      <c r="G24" s="8">
-        <v>0</v>
-      </c>
-      <c r="H24" s="7">
-        <v>0</v>
-      </c>
-      <c r="I24" s="4">
-        <v>1</v>
-      </c>
-      <c r="J24" s="4">
-        <v>1</v>
-      </c>
-      <c r="K24" s="6">
-        <v>0</v>
-      </c>
-      <c r="L24" t="s">
-        <v>19</v>
-      </c>
-      <c r="M24" s="3">
-        <v>0</v>
-      </c>
-      <c r="N24" s="6">
-        <v>0</v>
-      </c>
-      <c r="O24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="P24" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q24" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T24" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C25" s="4">
-        <v>0</v>
-      </c>
-      <c r="D25" s="4">
-        <v>0</v>
-      </c>
-      <c r="E25" s="4">
-        <v>0</v>
-      </c>
-      <c r="F25" s="3">
-        <v>0</v>
-      </c>
-      <c r="G25" s="8">
-        <v>1</v>
-      </c>
-      <c r="H25" s="7">
-        <v>1</v>
-      </c>
-      <c r="I25" s="4">
-        <v>0</v>
-      </c>
-      <c r="J25" s="4">
-        <v>0</v>
-      </c>
-      <c r="K25" s="6">
-        <v>0</v>
-      </c>
-      <c r="L25" t="s">
-        <v>19</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="N25" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="O25" s="3">
-        <v>0</v>
-      </c>
-      <c r="P25" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q25" s="8">
-        <v>1</v>
-      </c>
-      <c r="R25" s="7">
-        <v>1</v>
-      </c>
-      <c r="S25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="T25" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C26" s="4">
-        <v>0</v>
-      </c>
-      <c r="D26" s="4">
-        <v>0</v>
-      </c>
-      <c r="E26" s="4">
-        <v>0</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1</v>
-      </c>
-      <c r="G26" s="8">
-        <v>0</v>
-      </c>
-      <c r="H26" s="7">
-        <v>0</v>
-      </c>
-      <c r="I26" s="4">
-        <v>0</v>
-      </c>
-      <c r="J26" s="4">
-        <v>0</v>
-      </c>
-      <c r="K26" s="6">
-        <v>1</v>
-      </c>
-      <c r="L26" t="s">
-        <v>19</v>
-      </c>
-      <c r="M26" s="3">
-        <v>1</v>
-      </c>
-      <c r="N26" s="6">
-        <v>1</v>
-      </c>
-      <c r="O26" s="3">
-        <v>1</v>
-      </c>
-      <c r="P26" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q26" s="8">
-        <v>0</v>
-      </c>
-      <c r="R26" s="7">
-        <v>0</v>
-      </c>
-      <c r="S26" s="3">
-        <v>1</v>
-      </c>
-      <c r="T26" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="4">
-        <v>0</v>
-      </c>
-      <c r="D27" s="4">
-        <v>0</v>
-      </c>
-      <c r="E27" s="4">
-        <v>1</v>
-      </c>
-      <c r="F27" s="3">
-        <v>0</v>
-      </c>
-      <c r="G27" s="8">
-        <v>0</v>
-      </c>
-      <c r="H27" s="7">
-        <v>1</v>
-      </c>
-      <c r="I27" s="4">
-        <v>0</v>
-      </c>
-      <c r="J27" s="4">
-        <v>1</v>
-      </c>
-      <c r="K27" s="6">
-        <v>1</v>
-      </c>
-      <c r="L27" t="s">
-        <v>19</v>
-      </c>
-      <c r="M27" s="3">
-        <v>0</v>
-      </c>
-      <c r="N27" s="6">
-        <v>1</v>
-      </c>
-      <c r="O27" s="3">
-        <v>0</v>
-      </c>
-      <c r="P27" s="6">
-        <v>1</v>
-      </c>
-      <c r="Q27" s="8">
-        <v>0</v>
-      </c>
-      <c r="R27" s="7">
-        <v>1</v>
-      </c>
-      <c r="S27" s="3">
-        <v>0</v>
-      </c>
-      <c r="T27" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-      <c r="D28" s="4">
-        <v>1</v>
-      </c>
-      <c r="E28" s="4">
-        <v>0</v>
-      </c>
-      <c r="F28" s="3">
-        <v>0</v>
-      </c>
-      <c r="G28" s="8">
-        <v>0</v>
-      </c>
-      <c r="H28" s="7">
-        <v>0</v>
-      </c>
-      <c r="I28" s="4">
-        <v>0</v>
-      </c>
-      <c r="J28" s="4">
-        <v>0</v>
-      </c>
-      <c r="K28" s="6">
-        <v>0</v>
-      </c>
-      <c r="L28" s="5">
-        <v>1</v>
-      </c>
-      <c r="M28" s="3">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6">
-        <v>0</v>
-      </c>
-      <c r="O28" s="3">
-        <v>0</v>
-      </c>
-      <c r="P28" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q28" s="8">
-        <v>0</v>
-      </c>
-      <c r="R28" s="7">
-        <v>0</v>
-      </c>
-      <c r="S28" s="3">
-        <v>0</v>
-      </c>
-      <c r="T28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="4">
-        <v>0</v>
-      </c>
-      <c r="D29" s="4">
-        <v>0</v>
-      </c>
-      <c r="E29" s="4">
-        <v>0</v>
-      </c>
-      <c r="F29" s="3">
-        <v>0</v>
-      </c>
-      <c r="G29" s="8">
-        <v>0</v>
-      </c>
-      <c r="H29" s="7">
-        <v>0</v>
-      </c>
-      <c r="I29" s="4">
+      <c r="H36">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I36">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="J29" s="4">
-        <v>3</v>
-      </c>
-      <c r="K29" s="6">
-        <v>0</v>
-      </c>
-      <c r="L29" s="5">
-        <v>0</v>
-      </c>
-      <c r="M29" s="3">
-        <v>0</v>
-      </c>
-      <c r="N29" s="6">
-        <v>0</v>
-      </c>
-      <c r="O29" s="3">
-        <v>0</v>
-      </c>
-      <c r="P29" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q29" s="8">
-        <v>0</v>
-      </c>
-      <c r="R29" s="7">
-        <v>0</v>
-      </c>
-      <c r="S29" s="3">
-        <v>0</v>
-      </c>
-      <c r="T29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="4">
-        <v>0</v>
-      </c>
-      <c r="D30" s="4">
-        <v>0</v>
-      </c>
-      <c r="E30" s="4">
-        <v>0</v>
-      </c>
-      <c r="F30" s="3">
-        <v>0</v>
-      </c>
-      <c r="G30" s="8">
-        <v>10</v>
-      </c>
-      <c r="H30" s="7">
-        <v>10</v>
-      </c>
-      <c r="I30" s="4">
-        <v>0</v>
-      </c>
-      <c r="J30" s="4">
-        <v>0</v>
-      </c>
-      <c r="K30" s="6">
-        <v>0</v>
-      </c>
-      <c r="L30" s="5">
-        <v>0</v>
-      </c>
-      <c r="M30" s="3">
-        <v>0</v>
-      </c>
-      <c r="N30" s="6">
-        <v>0</v>
-      </c>
-      <c r="O30" s="3">
-        <v>0</v>
-      </c>
-      <c r="P30" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q30" s="8">
-        <v>10</v>
-      </c>
-      <c r="R30" s="7">
-        <v>10</v>
-      </c>
-      <c r="S30" s="3">
-        <v>0</v>
-      </c>
-      <c r="T30" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="4">
-        <v>0</v>
-      </c>
-      <c r="D31" s="4">
-        <v>0</v>
-      </c>
-      <c r="E31" s="4">
-        <v>0</v>
-      </c>
-      <c r="F31" s="3">
-        <v>12</v>
-      </c>
-      <c r="G31" s="8">
-        <v>0</v>
-      </c>
-      <c r="H31" s="7">
-        <v>0</v>
-      </c>
-      <c r="I31" s="4">
-        <v>0</v>
-      </c>
-      <c r="J31" s="4">
-        <v>0</v>
-      </c>
-      <c r="K31" s="6">
-        <v>12</v>
-      </c>
-      <c r="L31" s="5">
-        <v>0</v>
-      </c>
-      <c r="M31" s="3">
-        <v>12</v>
-      </c>
-      <c r="N31" s="6">
-        <v>12</v>
-      </c>
-      <c r="O31" s="3">
-        <v>12</v>
-      </c>
-      <c r="P31" s="6">
-        <v>12</v>
-      </c>
-      <c r="Q31" s="8">
-        <v>0</v>
-      </c>
-      <c r="R31" s="7">
-        <v>0</v>
-      </c>
-      <c r="S31" s="3">
-        <v>12</v>
-      </c>
-      <c r="T31" s="6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:35" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C32" s="4">
-        <v>0</v>
-      </c>
-      <c r="D32" s="4">
-        <v>0</v>
-      </c>
-      <c r="E32" s="4">
-        <v>5</v>
-      </c>
-      <c r="F32" s="3">
-        <v>0</v>
-      </c>
-      <c r="G32" s="8">
-        <v>0</v>
-      </c>
-      <c r="H32" s="7">
-        <v>5</v>
-      </c>
-      <c r="I32" s="4">
-        <v>0</v>
-      </c>
-      <c r="J32" s="4">
-        <v>5</v>
-      </c>
-      <c r="K32" s="6">
-        <v>5</v>
-      </c>
-      <c r="L32" s="5">
-        <v>0</v>
-      </c>
-      <c r="M32" s="3">
-        <v>0</v>
-      </c>
-      <c r="N32" s="6">
-        <v>5</v>
-      </c>
-      <c r="O32" s="3">
-        <v>0</v>
-      </c>
-      <c r="P32" s="6">
-        <v>5</v>
-      </c>
-      <c r="Q32" s="8">
-        <v>0</v>
-      </c>
-      <c r="R32" s="7">
-        <v>5</v>
-      </c>
-      <c r="S32" s="3">
-        <v>0</v>
-      </c>
-      <c r="T32" s="6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="4">
-        <v>0</v>
-      </c>
-      <c r="D34" s="4">
-        <v>0</v>
-      </c>
-      <c r="E34" s="4">
-        <v>0</v>
-      </c>
-      <c r="F34" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="4">
-        <v>1</v>
-      </c>
-      <c r="J34" s="4">
-        <v>1</v>
-      </c>
-      <c r="K34" s="6">
-        <v>0</v>
-      </c>
-      <c r="L34" t="s">
-        <v>19</v>
-      </c>
-      <c r="M34" s="4">
-        <v>0</v>
-      </c>
-      <c r="N34" s="4">
-        <v>0</v>
-      </c>
-      <c r="O34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="P34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="R34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S34" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T34" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4">
-        <v>0</v>
-      </c>
-      <c r="D35" s="4">
-        <v>0</v>
-      </c>
-      <c r="E35" s="4">
-        <v>0</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="8">
-        <v>1</v>
-      </c>
-      <c r="H35" s="7">
-        <v>1</v>
-      </c>
-      <c r="I35" s="4">
-        <v>0</v>
-      </c>
-      <c r="J35" s="4">
-        <v>0</v>
-      </c>
-      <c r="K35" s="6">
-        <v>0</v>
-      </c>
-      <c r="L35" t="s">
-        <v>19</v>
-      </c>
-      <c r="M35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="N35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="O35" s="4">
-        <v>0</v>
-      </c>
-      <c r="P35" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q35" s="4">
-        <v>1</v>
-      </c>
-      <c r="R35" s="4">
-        <v>1</v>
-      </c>
-      <c r="S35" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="T35" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>5</v>
-      </c>
-      <c r="C36" s="4">
-        <v>0</v>
-      </c>
-      <c r="D36" s="4">
-        <v>0</v>
-      </c>
-      <c r="E36" s="4">
-        <v>0</v>
-      </c>
-      <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="7">
-        <v>0</v>
-      </c>
-      <c r="I36" s="4">
-        <v>0</v>
-      </c>
-      <c r="J36" s="4">
-        <v>0</v>
-      </c>
-      <c r="K36" s="6">
-        <v>1</v>
-      </c>
-      <c r="L36" t="s">
-        <v>19</v>
-      </c>
-      <c r="M36" s="4">
-        <v>1</v>
-      </c>
-      <c r="N36" s="4">
-        <v>1</v>
-      </c>
-      <c r="O36" s="4">
-        <v>1</v>
-      </c>
-      <c r="P36" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q36" s="4">
-        <v>0</v>
-      </c>
-      <c r="R36" s="4">
-        <v>0</v>
-      </c>
-      <c r="S36" s="4">
-        <v>1</v>
-      </c>
-      <c r="T36" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>6</v>
-      </c>
-      <c r="C37" s="4">
-        <v>0</v>
-      </c>
-      <c r="D37" s="4">
-        <v>0</v>
-      </c>
-      <c r="E37" s="4">
-        <v>1</v>
-      </c>
-      <c r="F37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="G37" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="7">
-        <v>1</v>
-      </c>
-      <c r="I37" s="4">
-        <v>0</v>
-      </c>
-      <c r="J37" s="4">
-        <v>1</v>
-      </c>
-      <c r="K37" s="6">
-        <v>1</v>
-      </c>
-      <c r="L37" t="s">
-        <v>19</v>
-      </c>
-      <c r="M37" s="4">
-        <v>0</v>
-      </c>
-      <c r="N37" s="4">
-        <v>1</v>
-      </c>
-      <c r="O37" s="4">
-        <v>0</v>
-      </c>
-      <c r="P37" s="4">
-        <v>1</v>
-      </c>
-      <c r="Q37" s="4">
-        <v>0</v>
-      </c>
-      <c r="R37" s="4">
-        <v>1</v>
-      </c>
-      <c r="S37" s="4">
-        <v>0</v>
-      </c>
-      <c r="T37" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4">
-        <v>0</v>
-      </c>
-      <c r="D38" s="4">
-        <v>1</v>
-      </c>
-      <c r="E38" s="4">
-        <v>0</v>
-      </c>
-      <c r="F38" s="3">
-        <v>0</v>
-      </c>
-      <c r="G38" s="8">
-        <v>0</v>
-      </c>
-      <c r="H38" s="7">
-        <v>0</v>
-      </c>
-      <c r="I38" s="4">
-        <v>0</v>
-      </c>
-      <c r="J38" s="4">
-        <v>0</v>
-      </c>
-      <c r="K38" s="6">
-        <v>0</v>
-      </c>
-      <c r="L38" s="5">
-        <v>1</v>
-      </c>
-      <c r="M38" s="4">
-        <v>0</v>
-      </c>
-      <c r="N38" s="4">
-        <v>0</v>
-      </c>
-      <c r="O38" s="4">
-        <v>0</v>
-      </c>
-      <c r="P38" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q38" s="4">
-        <v>0</v>
-      </c>
-      <c r="R38" s="4">
-        <v>0</v>
-      </c>
-      <c r="S38" s="4">
-        <v>0</v>
-      </c>
-      <c r="T38" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="C39" s="4">
-        <v>0</v>
-      </c>
-      <c r="D39" s="4">
-        <v>0</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0</v>
-      </c>
-      <c r="F39" s="3">
-        <v>0</v>
-      </c>
-      <c r="G39" s="8">
-        <v>0</v>
-      </c>
-      <c r="H39" s="7">
-        <v>0</v>
-      </c>
-      <c r="I39" s="4">
-        <v>3</v>
-      </c>
-      <c r="J39" s="4">
-        <v>3</v>
-      </c>
-      <c r="K39" s="6">
-        <v>0</v>
-      </c>
-      <c r="L39" s="5">
-        <v>0</v>
-      </c>
-      <c r="M39" s="4">
-        <v>0</v>
-      </c>
-      <c r="N39" s="4">
-        <v>0</v>
-      </c>
-      <c r="O39" s="4">
-        <v>0</v>
-      </c>
-      <c r="P39" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q39" s="4">
-        <v>0</v>
-      </c>
-      <c r="R39" s="4">
-        <v>0</v>
-      </c>
-      <c r="S39" s="4">
-        <v>0</v>
-      </c>
-      <c r="T39" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>8</v>
-      </c>
-      <c r="C40" s="4">
-        <v>0</v>
-      </c>
-      <c r="D40" s="4">
-        <v>0</v>
-      </c>
-      <c r="E40" s="4">
-        <v>0</v>
-      </c>
-      <c r="F40" s="3">
-        <v>0</v>
-      </c>
-      <c r="G40" s="8">
-        <v>10</v>
-      </c>
-      <c r="H40" s="7">
-        <v>10</v>
-      </c>
-      <c r="I40" s="4">
-        <v>0</v>
-      </c>
-      <c r="J40" s="4">
-        <v>0</v>
-      </c>
-      <c r="K40" s="6">
-        <v>0</v>
-      </c>
-      <c r="L40" s="5">
-        <v>0</v>
-      </c>
-      <c r="M40" s="4">
-        <v>0</v>
-      </c>
-      <c r="N40" s="4">
-        <v>0</v>
-      </c>
-      <c r="O40" s="4">
-        <v>0</v>
-      </c>
-      <c r="P40" s="4">
-        <v>0</v>
-      </c>
-      <c r="Q40" s="4">
-        <v>10</v>
-      </c>
-      <c r="R40" s="4">
-        <v>10</v>
-      </c>
-      <c r="S40" s="4">
-        <v>0</v>
-      </c>
-      <c r="T40" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>9</v>
-      </c>
-      <c r="C41" s="4">
-        <v>0</v>
-      </c>
-      <c r="D41" s="4">
-        <v>0</v>
-      </c>
-      <c r="E41" s="4">
-        <v>0</v>
-      </c>
-      <c r="F41" s="3">
-        <v>12</v>
-      </c>
-      <c r="G41" s="8">
-        <v>0</v>
-      </c>
-      <c r="H41" s="7">
-        <v>0</v>
-      </c>
-      <c r="I41" s="4">
-        <v>0</v>
-      </c>
-      <c r="J41" s="4">
-        <v>0</v>
-      </c>
-      <c r="K41" s="6">
-        <v>12</v>
-      </c>
-      <c r="L41" s="5">
-        <v>0</v>
-      </c>
-      <c r="M41" s="4">
-        <v>12</v>
-      </c>
-      <c r="N41" s="4">
-        <v>12</v>
-      </c>
-      <c r="O41" s="4">
-        <v>12</v>
-      </c>
-      <c r="P41" s="4">
-        <v>12</v>
-      </c>
-      <c r="Q41" s="4">
-        <v>0</v>
-      </c>
-      <c r="R41" s="4">
-        <v>0</v>
-      </c>
-      <c r="S41" s="4">
-        <v>12</v>
-      </c>
-      <c r="T41" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C42" s="4">
-        <v>0</v>
-      </c>
-      <c r="D42" s="4">
-        <v>0</v>
-      </c>
-      <c r="E42" s="4">
-        <v>5</v>
-      </c>
-      <c r="F42" s="3">
-        <v>0</v>
-      </c>
-      <c r="G42" s="8">
-        <v>0</v>
-      </c>
-      <c r="H42" s="7">
-        <v>5</v>
-      </c>
-      <c r="I42" s="4">
-        <v>0</v>
-      </c>
-      <c r="J42" s="4">
-        <v>5</v>
-      </c>
-      <c r="K42" s="6">
-        <v>5</v>
-      </c>
-      <c r="L42" s="5">
-        <v>0</v>
-      </c>
-      <c r="M42" s="4">
-        <v>0</v>
-      </c>
-      <c r="N42" s="4">
-        <v>5</v>
-      </c>
-      <c r="O42" s="4">
-        <v>0</v>
-      </c>
-      <c r="P42" s="4">
-        <v>5</v>
-      </c>
-      <c r="Q42" s="4">
-        <v>0</v>
-      </c>
-      <c r="R42" s="4">
-        <v>5</v>
-      </c>
-      <c r="S42" s="4">
-        <v>0</v>
-      </c>
-      <c r="T42" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>17</v>
+      <c r="K36">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>